<commit_message>
2019 12 5 基本结束
</commit_message>
<xml_diff>
--- a/app/public/model.xlsx
+++ b/app/public/model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18120"/>
+    <workbookView windowWidth="26210" windowHeight="9220"/>
   </bookViews>
   <sheets>
     <sheet name="测区一数据" sheetId="1" r:id="rId1"/>
@@ -16,21 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
   <si>
     <t>测区一数据</t>
   </si>
   <si>
-    <t>测试地点:</t>
+    <t>项目名称:</t>
   </si>
   <si>
-    <t>&lt;%=_data_.position%&gt;</t>
+    <t>&lt;%=_data_.projectname%&gt;</t>
   </si>
   <si>
-    <t>待测结构名称：</t>
+    <t>工程名称：</t>
   </si>
   <si>
-    <t>&lt;%=_data_.name%&gt;</t>
+    <t>&lt;%=_data_.egineername%&gt;</t>
   </si>
   <si>
     <t>测量时间</t>
@@ -39,28 +39,10 @@
     <t>&lt;%=_data_.date%&gt;</t>
   </si>
   <si>
-    <t>温度:</t>
-  </si>
-  <si>
     <t>&lt;%=_data_.temperature%&gt;</t>
   </si>
   <si>
-    <t>湿度:</t>
-  </si>
-  <si>
-    <t>&lt;%=_data_.humidity%&gt;</t>
-  </si>
-  <si>
-    <t>待测区主筋D</t>
-  </si>
-  <si>
-    <t>22mm</t>
-  </si>
-  <si>
-    <t>待测结构使用时间U</t>
-  </si>
-  <si>
-    <t>5100天</t>
+    <t>&lt;%=_data_.howmanydays%&gt;</t>
   </si>
   <si>
     <t>测量点</t>
@@ -113,6 +95,9 @@
     <t>江苏省丹阳市</t>
   </si>
   <si>
+    <t>待测结构名称：</t>
+  </si>
+  <si>
     <t>XX桥梁</t>
   </si>
   <si>
@@ -125,7 +110,13 @@
     <t>湿度:55%</t>
   </si>
   <si>
+    <t>待测区主筋D</t>
+  </si>
+  <si>
     <t>10mm</t>
+  </si>
+  <si>
+    <t>待测结构使用时间U</t>
   </si>
   <si>
     <t>8760天</t>
@@ -165,11 +156,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -202,8 +193,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -219,38 +255,16 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,44 +278,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,7 +309,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,6 +325,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,7 +354,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,37 +462,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,31 +492,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,43 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,49 +528,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,6 +545,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -581,15 +581,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -601,15 +592,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,6 +628,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -660,10 +651,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -672,133 +663,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1272,13 +1263,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>533474</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1302,7 +1293,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1580515" y="990600"/>
+          <a:off x="1580515" y="768350"/>
           <a:ext cx="533400" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1316,13 +1307,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>361995</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>209579</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1346,7 +1337,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4255770" y="990600"/>
+          <a:off x="4255770" y="768350"/>
           <a:ext cx="323850" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1898,13 +1889,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="22.6272727272727" customWidth="1"/>
     <col min="2" max="2" width="37.7545454545455" customWidth="1"/>
@@ -1936,7 +1927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="17.5" spans="1:6">
+    <row r="3" ht="17.5" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1949,53 +1940,38 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" ht="20.1" customHeight="1" spans="1:4">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" ht="17.5" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="20.1" customHeight="1" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2008,12 +1984,12 @@
     <row r="9" spans="1:3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5"/>
@@ -2057,22 +2033,22 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3">
@@ -2113,7 +2089,7 @@
     <row r="30" spans="1:3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="5"/>
@@ -2122,12 +2098,12 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
@@ -2138,12 +2114,12 @@
     <row r="35" spans="1:3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5"/>
@@ -2192,12 +2168,12 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3">
@@ -2233,21 +2209,21 @@
     <row r="54" spans="1:3">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
+      <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="B56" s="6"/>
       <c r="C56" s="5"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="5"/>
-      <c r="B57" s="6"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="5"/>
     </row>
     <row r="58" spans="1:3">
@@ -2255,15 +2231,10 @@
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" ht="21" spans="1:3">
-      <c r="A60" s="7"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
+    <row r="59" ht="21" spans="1:3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2295,7 +2266,7 @@
   <sheetData>
     <row r="1" ht="25.5" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2303,16 +2274,16 @@
     </row>
     <row r="2" ht="17.5" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="17.5" spans="1:4">
@@ -2320,38 +2291,38 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" ht="17.5" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" ht="20.1" customHeight="1" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -3006,7 +2977,7 @@
     </row>
     <row r="65" ht="21" spans="1:3">
       <c r="A65" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B65" s="8">
         <f>AVERAGE(B6:B64)</f>

</xml_diff>